<commit_message>
added more logs for unity
</commit_message>
<xml_diff>
--- a/generators/errors.xlsx
+++ b/generators/errors.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F605"/>
+  <dimension ref="A1:F610"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26380,6 +26380,126 @@
       </c>
       <c r="F605" t="inlineStr"/>
     </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>testVersion-V02-24-01-21–15:57-GgPCN5YOxRMpHbi</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Unable to load asset: "assets/instructions/InstallIos.png".</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr"/>
+      <c r="D606" t="inlineStr">
+        <is>
+          <t>2024-01-21T16:00:46.670</t>
+        </is>
+      </c>
+      <c r="E606" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_0 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.0 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="F606" t="inlineStr"/>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>testVersion-V02-24-01-21–15:57-GgPCN5YOxRMpHbi</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Unable to load asset: "assets/instructions/InstallIos.png".</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr"/>
+      <c r="D607" t="inlineStr">
+        <is>
+          <t>2024-01-21T16:00:48.380</t>
+        </is>
+      </c>
+      <c r="E607" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_0 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.0 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="F607" t="inlineStr"/>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>testVersion-V02-24-01-21–16:01-tgsRoEZbTQAlhW1</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Unable to load asset: "assets/instructions/InstallIos.png".</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr"/>
+      <c r="D608" t="inlineStr">
+        <is>
+          <t>2024-01-21T16:01:47.679</t>
+        </is>
+      </c>
+      <c r="E608" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 14_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/14.0.3 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="F608" t="inlineStr"/>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>testVersion-V02-24-01-21–16:01-tgsRoEZbTQAlhW1</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>Unable to load asset: "assets/instructions/InstallIos.png".</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr"/>
+      <c r="D609" t="inlineStr">
+        <is>
+          <t>2024-01-21T16:03:22.697</t>
+        </is>
+      </c>
+      <c r="E609" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 14_6 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/14.0.3 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="F609" t="inlineStr"/>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>testVersion-V02-24-01-21–16:04-kQMhlaV4kJdkTWd</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Unable to load asset: "assets/instructions/InstallIos.png".</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr"/>
+      <c r="D610" t="inlineStr">
+        <is>
+          <t>2024-01-21T16:04:20.535</t>
+        </is>
+      </c>
+      <c r="E610" t="inlineStr">
+        <is>
+          <t>Mozilla/5.0 (iPhone; CPU iPhone OS 17_0_1 like Mac OS X) AppleWebKit/605.1.15 (KHTML, like Gecko) Version/17.0 Mobile/15E148 Safari/604.1</t>
+        </is>
+      </c>
+      <c r="F610" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>